<commit_message>
a1 need to put all together
</commit_message>
<xml_diff>
--- a/lef_plot9.xlsx
+++ b/lef_plot9.xlsx
@@ -2,23 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\downloaded\forest_analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA64117-94DF-4190-983B-47559EE206C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5146A81E-D615-432A-9FE8-E79D261810D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6C794430-0C18-4454-835E-2D085AB590D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C794430-0C18-4454-835E-2D085AB590D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Plot 9" sheetId="1" r:id="rId1"/>
-    <sheet name="Species_Slope_DRC" sheetId="2" r:id="rId2"/>
-    <sheet name="Data Key" sheetId="3" r:id="rId3"/>
+    <sheet name="tree24" sheetId="4" r:id="rId2"/>
+    <sheet name="Species_Slope_DRC" sheetId="2" r:id="rId3"/>
+    <sheet name="Data Key" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="183">
   <si>
     <t>Plot ID</t>
   </si>
@@ -588,6 +590,30 @@
   </si>
   <si>
     <t>volEQnum</t>
+  </si>
+  <si>
+    <t>Dead Tree Decay Class (1 - 5)</t>
+  </si>
+  <si>
+    <t>Phantom 4 inch DOB Height (ft) if Broken Top</t>
+  </si>
+  <si>
+    <t>Actual Height (ft) if Broken Top</t>
+  </si>
+  <si>
+    <t>Broken Top Diameter (in)</t>
+  </si>
+  <si>
+    <t>DBH Height (ft, if different from 4.5 ft/DRC)</t>
+  </si>
+  <si>
+    <t>ht</t>
+  </si>
+  <si>
+    <t>dib2at</t>
+  </si>
+  <si>
+    <t>dib in</t>
   </si>
 </sst>
 </file>
@@ -597,7 +623,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="###0.0;\-###0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1307,7 +1333,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1481,6 +1507,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1496,11 +1530,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1520,7 +1549,1574 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tree24!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dib in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tree24!$N$2:$N$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tree24!$O$2:$O$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>20.1937255859375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.88627815246582</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.68548583984375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.924393653869629</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.396261215209961</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.009604454040527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.715923309326172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.486467361450195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.302850723266602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.152651786804199</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.027126312255859</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.919919967651367</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.826301574707031</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.742681503295898</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.666291236877441</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.594975471496582</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.527040481567383</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.461148262023926</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.396241188049316</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.33154296875</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.266825675964355</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.202018737792969</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.13704776763916</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.071834564208984</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.006305694580078</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.940382957458496</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12.873992919921875</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.807058334350586</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.739502906799316</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.671252250671387</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12.602229118347168</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.532358169555664</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12.461565017700195</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.389771461486816</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12.316902160644531</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.24288272857666</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12.167635917663574</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.091087341308594</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.013160705566406</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11.933779716491699</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>11.852869033813477</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11.770353317260742</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11.6861572265625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11.60020637512207</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11.512423515319824</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11.422735214233398</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11.331066131591797</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11.23734188079834</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11.141488075256348</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>11.043429374694824</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10.943093299865723</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10.840405464172363</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10.735294342041016</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10.627686500549316</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10.517511367797852</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>10.404695510864258</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10.289169311523438</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>10.170864105224609</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10.049708366394043</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9.9256381988525391</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.7985820770263672</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.6684789657592773</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.5352621078491211</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9.3988685607910156</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.2592391967773438</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.1163120269775391</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.9700326919555664</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.820343017578125</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>8.6671943664550781</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8.5105323791503906</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.3503103256225586</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>8.1864862442016602</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.0190153121948242</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.8478631973266602</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.6729946136474609</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.4943790435791016</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.3119931221008301</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.1258144378662109</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.9358291625976563</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.7420282363891602</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.5444040298461914</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.3429622650146484</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.1377100944519043</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.9286661148071289</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.7158517837524414</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.4993019104003906</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.2790560722351074</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.0551638603210449</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.8276877403259277</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.5966958999633789</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.3622736930847168</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.12451171875</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.8835158348083496</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.6394081115722656</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.3923192024230957</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.1424002647399902</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.8898136615753174</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.6347389221191406</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.3773760795593262</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.117938756942749</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.8566651344299316</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1.5938084125518799</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1.3296496868133545</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.0644845962524414</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.79863625764846802</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.5324552059173584</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.26622676849365234</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A491-4CCB-8DA5-BE79958DAFE0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="382847776"/>
+        <c:axId val="382866016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="382847776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382866016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="382866016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="382847776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{258D4D98-2E6D-2402-B531-727EDCE1F5EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1581,6 +3177,7 @@
       <sheetName val="Sheet3"/>
     </sheetNames>
     <definedNames>
+      <definedName name="calcDib"/>
       <definedName name="calcMerchCubic"/>
       <definedName name="calcTotCubic"/>
       <definedName name="VolumeEquationNumber"/>
@@ -1589,6 +3186,27 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="getDibAdv"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1911,23 +3529,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D812436D-6A40-4A03-B64E-FFF3E6BAFEF7}">
-  <dimension ref="A1:K34"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="M1" sqref="M1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>166</v>
       </c>
@@ -1946,23 +3565,30 @@
       <c r="F1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="88" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="88" t="s">
-        <v>172</v>
-      </c>
-      <c r="J1" s="88" t="s">
-        <v>173</v>
-      </c>
-      <c r="K1" s="88" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>9</v>
       </c>
@@ -1979,27 +3605,13 @@
       <c r="F2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>61</v>
       </c>
-      <c r="H2" s="89">
-        <f>(PI() * (D2/2)^2) / 144</f>
-        <v>0.3490658503988659</v>
-      </c>
-      <c r="I2" s="90" cm="1">
-        <f t="array" ref="I2">[1]!calcTotCubic(1,16,K2,D2,G2)</f>
-        <v>8</v>
-      </c>
-      <c r="J2" cm="1">
-        <f t="array" ref="J2">[1]!calcMerchCubic(1,16,K2,D2,G2,4,0)</f>
-        <v>6.5</v>
-      </c>
-      <c r="K2" t="str" cm="1">
-        <f t="array" ref="K2">[1]!VolumeEquationNumber(1,16,1,C2,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="84"/>
+      <c r="N2" s="85"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>9</v>
       </c>
@@ -2016,27 +3628,13 @@
       <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <v>93</v>
       </c>
-      <c r="H3" s="89">
-        <f t="shared" ref="H3:H34" si="0">(PI() * (D3/2)^2) / 144</f>
-        <v>1.413771235654532</v>
-      </c>
-      <c r="I3" s="90" cm="1">
-        <f t="array" ref="I3">[1]!calcTotCubic(1,16,K3,D3,G3)</f>
-        <v>45.3</v>
-      </c>
-      <c r="J3" cm="1">
-        <f t="array" ref="J3">[1]!calcMerchCubic(1,16,K3,D3,G3,4,0)</f>
-        <v>42.3</v>
-      </c>
-      <c r="K3" t="str" cm="1">
-        <f t="array" ref="K3">[1]!VolumeEquationNumber(1,16,1,C3,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="84"/>
+      <c r="N3" s="85"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>9</v>
       </c>
@@ -2053,27 +3651,13 @@
       <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="6">
+      <c r="H4" s="6">
         <v>34</v>
       </c>
-      <c r="H4" s="89">
-        <f t="shared" si="0"/>
-        <v>0.2906518619961807</v>
-      </c>
-      <c r="I4" s="90" cm="1">
-        <f t="array" ref="I4">[1]!calcTotCubic(1,16,K4,D4,G4)</f>
-        <v>3.8</v>
-      </c>
-      <c r="J4" cm="1">
-        <f t="array" ref="J4">[1]!calcMerchCubic(1,16,K4,D4,G4,4,0)</f>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="K4" t="str" cm="1">
-        <f t="array" ref="K4">[1]!VolumeEquationNumber(1,16,1,C4,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="84"/>
+      <c r="N4" s="85"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>9</v>
       </c>
@@ -2090,27 +3674,13 @@
       <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <v>88</v>
       </c>
-      <c r="H5" s="89">
-        <f t="shared" si="0"/>
-        <v>1.3615749827120764</v>
-      </c>
-      <c r="I5" s="90" cm="1">
-        <f t="array" ref="I5">[1]!calcTotCubic(1,16,K5,D5,G5)</f>
-        <v>42.9</v>
-      </c>
-      <c r="J5" cm="1">
-        <f t="array" ref="J5">[1]!calcMerchCubic(1,16,K5,D5,G5,4,0)</f>
-        <v>40.4</v>
-      </c>
-      <c r="K5" t="str" cm="1">
-        <f t="array" ref="K5">[1]!VolumeEquationNumber(1,16,1,C5,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="84"/>
+      <c r="N5" s="85"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>9</v>
       </c>
@@ -2127,27 +3697,13 @@
       <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="6">
         <v>68</v>
       </c>
-      <c r="H6" s="89">
-        <f t="shared" si="0"/>
-        <v>0.38484510006474965</v>
-      </c>
-      <c r="I6" s="90" cm="1">
-        <f t="array" ref="I6">[1]!calcTotCubic(1,16,K6,D6,G6)</f>
-        <v>10.4</v>
-      </c>
-      <c r="J6" cm="1">
-        <f t="array" ref="J6">[1]!calcMerchCubic(1,16,K6,D6,G6,4,0)</f>
-        <v>8.4</v>
-      </c>
-      <c r="K6" t="str" cm="1">
-        <f t="array" ref="K6">[1]!VolumeEquationNumber(1,16,1,C6,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="84"/>
+      <c r="N6" s="85"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>9</v>
       </c>
@@ -2164,27 +3720,13 @@
       <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="6">
         <v>68</v>
       </c>
-      <c r="H7" s="89">
-        <f t="shared" si="0"/>
-        <v>0.27494389872823172</v>
-      </c>
-      <c r="I7" s="90" cm="1">
-        <f t="array" ref="I7">[1]!calcTotCubic(1,16,K7,D7,G7)</f>
-        <v>7.3</v>
-      </c>
-      <c r="J7" cm="1">
-        <f t="array" ref="J7">[1]!calcMerchCubic(1,16,K7,D7,G7,4,0)</f>
-        <v>5.4</v>
-      </c>
-      <c r="K7" t="str" cm="1">
-        <f t="array" ref="K7">[1]!VolumeEquationNumber(1,16,1,C7,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="84"/>
+      <c r="N7" s="85"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>9</v>
       </c>
@@ -2201,27 +3743,13 @@
       <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <v>78</v>
       </c>
-      <c r="H8" s="89">
-        <f t="shared" si="0"/>
-        <v>0.33183072403542185</v>
-      </c>
-      <c r="I8" s="90" cm="1">
-        <f t="array" ref="I8">[1]!calcTotCubic(1,16,K8,D8,G8)</f>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="J8" cm="1">
-        <f t="array" ref="J8">[1]!calcMerchCubic(1,16,K8,D8,G8,4,0)</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="K8" t="str" cm="1">
-        <f t="array" ref="K8">[1]!VolumeEquationNumber(1,16,1,C8,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="84"/>
+      <c r="N8" s="85"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9</v>
       </c>
@@ -2238,27 +3766,13 @@
       <c r="F9" s="6">
         <v>1</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="6">
         <v>71</v>
       </c>
-      <c r="H9" s="89">
-        <f t="shared" si="0"/>
-        <v>0.40338922336718935</v>
-      </c>
-      <c r="I9" s="90" cm="1">
-        <f t="array" ref="I9">[1]!calcTotCubic(1,16,K9,D9,G9)</f>
-        <v>10.9</v>
-      </c>
-      <c r="J9" cm="1">
-        <f t="array" ref="J9">[1]!calcMerchCubic(1,16,K9,D9,G9,4,0)</f>
-        <v>9.1</v>
-      </c>
-      <c r="K9" t="str" cm="1">
-        <f t="array" ref="K9">[1]!VolumeEquationNumber(1,16,1,C9,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="84"/>
+      <c r="N9" s="85"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2275,27 +3789,13 @@
       <c r="F10" s="6">
         <v>1</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="6">
         <v>82</v>
       </c>
-      <c r="H10" s="89">
-        <f t="shared" si="0"/>
-        <v>0.40338922336718935</v>
-      </c>
-      <c r="I10" s="90" cm="1">
-        <f t="array" ref="I10">[1]!calcTotCubic(1,16,K10,D10,G10)</f>
-        <v>12.8</v>
-      </c>
-      <c r="J10" cm="1">
-        <f t="array" ref="J10">[1]!calcMerchCubic(1,16,K10,D10,G10,4,0)</f>
-        <v>11.1</v>
-      </c>
-      <c r="K10" t="str" cm="1">
-        <f t="array" ref="K10">[1]!VolumeEquationNumber(1,16,1,C10,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="84"/>
+      <c r="N10" s="85"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -2312,27 +3812,13 @@
       <c r="F11" s="6">
         <v>1</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>55</v>
       </c>
-      <c r="H11" s="89">
-        <f t="shared" si="0"/>
-        <v>0.38484510006474965</v>
-      </c>
-      <c r="I11" s="90" cm="1">
-        <f t="array" ref="I11">[1]!calcTotCubic(1,16,K11,D11,G11)</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J11" cm="1">
-        <f t="array" ref="J11">[1]!calcMerchCubic(1,16,K11,D11,G11,4,0)</f>
-        <v>6.3</v>
-      </c>
-      <c r="K11" t="str" cm="1">
-        <f t="array" ref="K11">[1]!VolumeEquationNumber(1,16,1,C11,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="84"/>
+      <c r="N11" s="85"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -2349,27 +3835,13 @@
       <c r="F12" s="6">
         <v>1</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <v>76</v>
       </c>
-      <c r="H12" s="89">
-        <f t="shared" si="0"/>
-        <v>0.45165848549265752</v>
-      </c>
-      <c r="I12" s="90" cm="1">
-        <f t="array" ref="I12">[1]!calcTotCubic(1,16,K12,D12,G12)</f>
-        <v>13.1</v>
-      </c>
-      <c r="J12" cm="1">
-        <f t="array" ref="J12">[1]!calcMerchCubic(1,16,K12,D12,G12,4,0)</f>
-        <v>11.2</v>
-      </c>
-      <c r="K12" t="str" cm="1">
-        <f t="array" ref="K12">[1]!VolumeEquationNumber(1,16,1,C12,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="84"/>
+      <c r="N12" s="85"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -2386,27 +3858,25 @@
       <c r="F13" s="6">
         <v>2</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="6">
         <v>63</v>
       </c>
-      <c r="H13" s="89">
-        <f t="shared" si="0"/>
-        <v>0.25220007691318058</v>
-      </c>
-      <c r="I13" s="90" cm="1">
-        <f t="array" ref="I13">[1]!calcTotCubic(1,16,K13,D13,G13)</f>
-        <v>6.5</v>
-      </c>
-      <c r="J13" cm="1">
-        <f t="array" ref="J13">[1]!calcMerchCubic(1,16,K13,D13,G13,4,0)</f>
-        <v>5</v>
-      </c>
-      <c r="K13" t="str" cm="1">
-        <f t="array" ref="K13">[1]!VolumeEquationNumber(1,16,1,C13,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>23</v>
+      </c>
+      <c r="L13">
+        <v>43</v>
+      </c>
+      <c r="M13" s="84"/>
+      <c r="N13" s="85"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>9</v>
       </c>
@@ -2423,27 +3893,13 @@
       <c r="F14" s="6">
         <v>1</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <v>88</v>
       </c>
-      <c r="H14" s="89">
-        <f t="shared" si="0"/>
-        <v>0.54541539124822802</v>
-      </c>
-      <c r="I14" s="90" cm="1">
-        <f t="array" ref="I14">[1]!calcTotCubic(1,16,K14,D14,G14)</f>
-        <v>18.3</v>
-      </c>
-      <c r="J14" cm="1">
-        <f t="array" ref="J14">[1]!calcMerchCubic(1,16,K14,D14,G14,4,0)</f>
-        <v>17.2</v>
-      </c>
-      <c r="K14" t="str" cm="1">
-        <f t="array" ref="K14">[1]!VolumeEquationNumber(1,16,1,C14,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14" s="84"/>
+      <c r="N14" s="85"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>9</v>
       </c>
@@ -2460,27 +3916,13 @@
       <c r="F15" s="6">
         <v>1</v>
       </c>
-      <c r="G15" s="6">
+      <c r="H15" s="6">
         <v>69</v>
       </c>
-      <c r="H15" s="89">
-        <f t="shared" si="0"/>
-        <v>0.25967226777328134</v>
-      </c>
-      <c r="I15" s="90" cm="1">
-        <f t="array" ref="I15">[1]!calcTotCubic(1,16,K15,D15,G15)</f>
-        <v>7.1</v>
-      </c>
-      <c r="J15" cm="1">
-        <f t="array" ref="J15">[1]!calcMerchCubic(1,16,K15,D15,G15,4,0)</f>
-        <v>5.4</v>
-      </c>
-      <c r="K15" t="str" cm="1">
-        <f t="array" ref="K15">[1]!VolumeEquationNumber(1,16,1,C15,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15" s="84"/>
+      <c r="N15" s="85"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>9</v>
       </c>
@@ -2497,27 +3939,13 @@
       <c r="F16" s="6">
         <v>1</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H16" s="6">
         <v>51</v>
       </c>
-      <c r="H16" s="89">
-        <f t="shared" si="0"/>
-        <v>0.15904312808798329</v>
-      </c>
-      <c r="I16" s="90" cm="1">
-        <f t="array" ref="I16">[1]!calcTotCubic(1,16,K16,D16,G16)</f>
-        <v>3.2</v>
-      </c>
-      <c r="J16" cm="1">
-        <f t="array" ref="J16">[1]!calcMerchCubic(1,16,K16,D16,G16,4,0)</f>
-        <v>1.6</v>
-      </c>
-      <c r="K16" t="str" cm="1">
-        <f t="array" ref="K16">[1]!VolumeEquationNumber(1,16,1,C16,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="84"/>
+      <c r="N16" s="85"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>9</v>
       </c>
@@ -2532,25 +3960,11 @@
       <c r="F17" s="6">
         <v>0</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="89">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="90" t="str" cm="1">
-        <f t="array" ref="I17">[1]!calcTotCubic(1,16,K17,D17,G17)</f>
-        <v>#DBH&lt;1!</v>
-      </c>
-      <c r="J17" t="str" cm="1">
-        <f t="array" ref="J17">[1]!calcMerchCubic(1,16,K17,D17,G17,4,0)</f>
-        <v>#DBH&lt;1!</v>
-      </c>
-      <c r="K17" t="str" cm="1">
-        <f t="array" ref="K17">[1]!VolumeEquationNumber(1,16,1,C17,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="6"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="85"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>9</v>
       </c>
@@ -2567,27 +3981,13 @@
       <c r="F18" s="6">
         <v>1</v>
       </c>
-      <c r="G18" s="6">
+      <c r="H18" s="6">
         <v>88</v>
       </c>
-      <c r="H18" s="89">
-        <f t="shared" si="0"/>
-        <v>1.0088003076527223</v>
-      </c>
-      <c r="I18" s="90" cm="1">
-        <f t="array" ref="I18">[1]!calcTotCubic(1,16,K18,D18,G18)</f>
-        <v>31.7</v>
-      </c>
-      <c r="J18" cm="1">
-        <f t="array" ref="J18">[1]!calcMerchCubic(1,16,K18,D18,G18,4,0)</f>
-        <v>27.9</v>
-      </c>
-      <c r="K18" t="str" cm="1">
-        <f t="array" ref="K18">[1]!VolumeEquationNumber(1,16,1,C18,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18" s="84"/>
+      <c r="N18" s="85"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>9</v>
       </c>
@@ -2604,27 +4004,16 @@
       <c r="F19" s="6">
         <v>1</v>
       </c>
-      <c r="G19" s="6">
+      <c r="H19" s="6">
         <v>75</v>
       </c>
-      <c r="H19" s="89">
-        <f t="shared" si="0"/>
-        <v>0.46163958715250009</v>
-      </c>
-      <c r="I19" s="90" cm="1">
-        <f t="array" ref="I19">[1]!calcTotCubic(1,16,K19,D19,G19)</f>
-        <v>13.1</v>
-      </c>
-      <c r="J19" cm="1">
-        <f t="array" ref="J19">[1]!calcMerchCubic(1,16,K19,D19,G19,4,0)</f>
-        <v>11.2</v>
-      </c>
-      <c r="K19" t="str" cm="1">
-        <f t="array" ref="K19">[1]!VolumeEquationNumber(1,16,1,C19,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M19" s="84"/>
+      <c r="N19" s="85"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>9</v>
       </c>
@@ -2641,27 +4030,13 @@
       <c r="F20" s="6">
         <v>1</v>
       </c>
-      <c r="G20" s="6">
+      <c r="H20" s="6">
         <v>83</v>
       </c>
-      <c r="H20" s="89">
-        <f t="shared" si="0"/>
-        <v>0.68416906678177702</v>
-      </c>
-      <c r="I20" s="90" cm="1">
-        <f t="array" ref="I20">[1]!calcTotCubic(1,16,K20,D20,G20)</f>
-        <v>21</v>
-      </c>
-      <c r="J20" cm="1">
-        <f t="array" ref="J20">[1]!calcMerchCubic(1,16,K20,D20,G20,4,0)</f>
-        <v>20</v>
-      </c>
-      <c r="K20" t="str" cm="1">
-        <f t="array" ref="K20">[1]!VolumeEquationNumber(1,16,1,C20,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" s="84"/>
+      <c r="N20" s="85"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>9</v>
       </c>
@@ -2678,27 +4053,13 @@
       <c r="F21" s="6">
         <v>1</v>
       </c>
-      <c r="G21" s="6">
+      <c r="H21" s="6">
         <v>42</v>
       </c>
-      <c r="H21" s="89">
-        <f t="shared" si="0"/>
-        <v>0.19634954084936207</v>
-      </c>
-      <c r="I21" s="90" cm="1">
-        <f t="array" ref="I21">[1]!calcTotCubic(1,16,K21,D21,G21)</f>
-        <v>3.4</v>
-      </c>
-      <c r="J21" cm="1">
-        <f t="array" ref="J21">[1]!calcMerchCubic(1,16,K21,D21,G21,4,0)</f>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="K21" t="str" cm="1">
-        <f t="array" ref="K21">[1]!VolumeEquationNumber(1,16,1,C21,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21" s="84"/>
+      <c r="N21" s="85"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>9</v>
       </c>
@@ -2715,27 +4076,13 @@
       <c r="F22" s="6">
         <v>1</v>
       </c>
-      <c r="G22" s="6">
+      <c r="H22" s="6">
         <v>96</v>
       </c>
-      <c r="H22" s="89">
-        <f t="shared" si="0"/>
-        <v>1.0843403393406019</v>
-      </c>
-      <c r="I22" s="90" cm="1">
-        <f t="array" ref="I22">[1]!calcTotCubic(1,16,K22,D22,G22)</f>
-        <v>37.299999999999997</v>
-      </c>
-      <c r="J22" cm="1">
-        <f t="array" ref="J22">[1]!calcMerchCubic(1,16,K22,D22,G22,4,0)</f>
-        <v>34.200000000000003</v>
-      </c>
-      <c r="K22" t="str" cm="1">
-        <f t="array" ref="K22">[1]!VolumeEquationNumber(1,16,1,C22,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22" s="84"/>
+      <c r="N22" s="85"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>9</v>
       </c>
@@ -2752,27 +4099,13 @@
       <c r="F23" s="6">
         <v>1</v>
       </c>
-      <c r="G23" s="6">
+      <c r="H23" s="6">
         <v>53</v>
       </c>
-      <c r="H23" s="89">
-        <f t="shared" si="0"/>
-        <v>0.31503192998497648</v>
-      </c>
-      <c r="I23" s="90" cm="1">
-        <f t="array" ref="I23">[1]!calcTotCubic(1,16,K23,D23,G23)</f>
-        <v>6.2</v>
-      </c>
-      <c r="J23" cm="1">
-        <f t="array" ref="J23">[1]!calcMerchCubic(1,16,K23,D23,G23,4,0)</f>
-        <v>4.3</v>
-      </c>
-      <c r="K23" t="str" cm="1">
-        <f t="array" ref="K23">[1]!VolumeEquationNumber(1,16,1,C23,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23" s="84"/>
+      <c r="N23" s="85"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>9</v>
       </c>
@@ -2789,27 +4122,13 @@
       <c r="F24" s="6">
         <v>1</v>
       </c>
-      <c r="G24" s="6">
+      <c r="H24" s="6">
         <v>41</v>
       </c>
-      <c r="H24" s="89">
-        <f t="shared" si="0"/>
-        <v>0.17104226669544426</v>
-      </c>
-      <c r="I24" s="90" cm="1">
-        <f t="array" ref="I24">[1]!calcTotCubic(1,16,K24,D24,G24)</f>
-        <v>2.9</v>
-      </c>
-      <c r="J24" cm="1">
-        <f t="array" ref="J24">[1]!calcMerchCubic(1,16,K24,D24,G24,4,0)</f>
-        <v>1.6</v>
-      </c>
-      <c r="K24" t="str" cm="1">
-        <f t="array" ref="K24">[1]!VolumeEquationNumber(1,16,1,C24,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24" s="84"/>
+      <c r="N24" s="85"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>9</v>
       </c>
@@ -2826,27 +4145,13 @@
       <c r="F25" s="6">
         <v>1</v>
       </c>
-      <c r="G25" s="6">
+      <c r="H25" s="6">
         <v>107</v>
       </c>
-      <c r="H25" s="89">
-        <f t="shared" si="0"/>
-        <v>1.747565455098447</v>
-      </c>
-      <c r="I25" s="90" cm="1">
-        <f t="array" ref="I25">[1]!calcTotCubic(1,16,K25,D25,G25)</f>
-        <v>63.7</v>
-      </c>
-      <c r="J25" cm="1">
-        <f t="array" ref="J25">[1]!calcMerchCubic(1,16,K25,D25,G25,4,0)</f>
-        <v>57.7</v>
-      </c>
-      <c r="K25" t="str" cm="1">
-        <f t="array" ref="K25">[1]!VolumeEquationNumber(1,16,1,C25,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25" s="84"/>
+      <c r="N25" s="85"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>9</v>
       </c>
@@ -2863,27 +4168,13 @@
       <c r="F26" s="6">
         <v>1</v>
       </c>
-      <c r="G26" s="6">
+      <c r="H26" s="6">
         <v>56</v>
       </c>
-      <c r="H26" s="89">
-        <f t="shared" si="0"/>
-        <v>0.40338922336718935</v>
-      </c>
-      <c r="I26" s="90" cm="1">
-        <f t="array" ref="I26">[1]!calcTotCubic(1,16,K26,D26,G26)</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="J26" cm="1">
-        <f t="array" ref="J26">[1]!calcMerchCubic(1,16,K26,D26,G26,4,0)</f>
-        <v>6.5</v>
-      </c>
-      <c r="K26" t="str" cm="1">
-        <f t="array" ref="K26">[1]!VolumeEquationNumber(1,16,1,C26,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26" s="84"/>
+      <c r="N26" s="85"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>9</v>
       </c>
@@ -2900,27 +4191,13 @@
       <c r="F27" s="6">
         <v>1</v>
       </c>
-      <c r="G27" s="6">
+      <c r="H27" s="6">
         <v>50</v>
       </c>
-      <c r="H27" s="89">
-        <f t="shared" si="0"/>
-        <v>0.48192903970693429</v>
-      </c>
-      <c r="I27" s="90" cm="1">
-        <f t="array" ref="I27">[1]!calcTotCubic(1,16,K27,D27,G27)</f>
-        <v>9</v>
-      </c>
-      <c r="J27" cm="1">
-        <f t="array" ref="J27">[1]!calcMerchCubic(1,16,K27,D27,G27,4,0)</f>
-        <v>7.7</v>
-      </c>
-      <c r="K27" t="str" cm="1">
-        <f t="array" ref="K27">[1]!VolumeEquationNumber(1,16,1,C27,0)</f>
-        <v>I00FW2W202</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27" s="84"/>
+      <c r="N27" s="85"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>9</v>
       </c>
@@ -2937,27 +4214,13 @@
       <c r="F28" s="6">
         <v>1</v>
       </c>
-      <c r="G28" s="6">
+      <c r="H28" s="6">
         <v>96</v>
       </c>
-      <c r="H28" s="89">
-        <f t="shared" si="0"/>
-        <v>1.0690141668465267</v>
-      </c>
-      <c r="I28" s="90" cm="1">
-        <f t="array" ref="I28">[1]!calcTotCubic(1,16,K28,D28,G28)</f>
-        <v>36.799999999999997</v>
-      </c>
-      <c r="J28" cm="1">
-        <f t="array" ref="J28">[1]!calcMerchCubic(1,16,K28,D28,G28,4,0)</f>
-        <v>34.200000000000003</v>
-      </c>
-      <c r="K28" t="str" cm="1">
-        <f t="array" ref="K28">[1]!VolumeEquationNumber(1,16,1,C28,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28" s="84"/>
+      <c r="N28" s="85"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>9</v>
       </c>
@@ -2974,27 +4237,13 @@
       <c r="F29" s="6">
         <v>1</v>
       </c>
-      <c r="G29" s="6">
+      <c r="H29" s="6">
         <v>90</v>
       </c>
-      <c r="H29" s="89">
-        <f t="shared" si="0"/>
-        <v>1.6512996385431347</v>
-      </c>
-      <c r="I29" s="90" cm="1">
-        <f t="array" ref="I29">[1]!calcTotCubic(1,16,K29,D29,G29)</f>
-        <v>49.6</v>
-      </c>
-      <c r="J29" cm="1">
-        <f t="array" ref="J29">[1]!calcMerchCubic(1,16,K29,D29,G29,4,0)</f>
-        <v>45.1</v>
-      </c>
-      <c r="K29" t="str" cm="1">
-        <f t="array" ref="K29">[1]!VolumeEquationNumber(1,16,1,C29,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M29" s="84"/>
+      <c r="N29" s="85"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>9</v>
       </c>
@@ -3011,27 +4260,13 @@
       <c r="F30" s="6">
         <v>1</v>
       </c>
-      <c r="G30" s="6">
+      <c r="H30" s="6">
         <v>93</v>
       </c>
-      <c r="H30" s="89">
-        <f t="shared" si="0"/>
-        <v>1.1309733552923256</v>
-      </c>
-      <c r="I30" s="90" cm="1">
-        <f t="array" ref="I30">[1]!calcTotCubic(1,16,K30,D30,G30)</f>
-        <v>37.299999999999997</v>
-      </c>
-      <c r="J30" cm="1">
-        <f t="array" ref="J30">[1]!calcMerchCubic(1,16,K30,D30,G30,4,0)</f>
-        <v>33.4</v>
-      </c>
-      <c r="K30" t="str" cm="1">
-        <f t="array" ref="K30">[1]!VolumeEquationNumber(1,16,1,C30,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30" s="84"/>
+      <c r="N30" s="85"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>9</v>
       </c>
@@ -3048,27 +4283,13 @@
       <c r="F31" s="6">
         <v>1</v>
       </c>
-      <c r="G31" s="6">
+      <c r="H31" s="6">
         <v>93</v>
       </c>
-      <c r="H31" s="89">
-        <f t="shared" si="0"/>
-        <v>1.413771235654532</v>
-      </c>
-      <c r="I31" s="90" cm="1">
-        <f t="array" ref="I31">[1]!calcTotCubic(1,16,K31,D31,G31)</f>
-        <v>45.3</v>
-      </c>
-      <c r="J31" cm="1">
-        <f t="array" ref="J31">[1]!calcMerchCubic(1,16,K31,D31,G31,4,0)</f>
-        <v>42.3</v>
-      </c>
-      <c r="K31" t="str" cm="1">
-        <f t="array" ref="K31">[1]!VolumeEquationNumber(1,16,1,C31,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M31" s="84"/>
+      <c r="N31" s="85"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>9</v>
       </c>
@@ -3085,27 +4306,13 @@
       <c r="F32" s="6">
         <v>1</v>
       </c>
-      <c r="G32" s="6">
+      <c r="H32" s="6">
         <v>26</v>
       </c>
-      <c r="H32" s="89">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="90" t="str" cm="1">
-        <f t="array" ref="I32">[1]!calcTotCubic(1,16,K32,D32,G32)</f>
-        <v>#DBH&lt;1!</v>
-      </c>
-      <c r="J32" t="str" cm="1">
-        <f t="array" ref="J32">[1]!calcMerchCubic(1,16,K32,D32,G32,4,0)</f>
-        <v>#DBH&lt;1!</v>
-      </c>
-      <c r="K32" t="str" cm="1">
-        <f t="array" ref="K32">[1]!VolumeEquationNumber(1,16,1,C32,0)</f>
-        <v>102DVEW106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M32" s="84"/>
+      <c r="N32" s="85"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>9</v>
       </c>
@@ -3122,27 +4329,13 @@
       <c r="F33" s="6">
         <v>1</v>
       </c>
-      <c r="G33" s="6">
+      <c r="H33" s="6">
         <v>86</v>
       </c>
-      <c r="H33" s="89">
-        <f t="shared" si="0"/>
-        <v>0.58992128717408343</v>
-      </c>
-      <c r="I33" s="90" cm="1">
-        <f t="array" ref="I33">[1]!calcTotCubic(1,16,K33,D33,G33)</f>
-        <v>19.100000000000001</v>
-      </c>
-      <c r="J33" cm="1">
-        <f t="array" ref="J33">[1]!calcMerchCubic(1,16,K33,D33,G33,4,0)</f>
-        <v>16.899999999999999</v>
-      </c>
-      <c r="K33" t="str" cm="1">
-        <f t="array" ref="K33">[1]!VolumeEquationNumber(1,16,1,C33,0)</f>
-        <v>I00FW2W073</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33" s="84"/>
+      <c r="N33" s="85"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>9</v>
       </c>
@@ -3159,31 +4352,1532 @@
       <c r="F34" s="6">
         <v>1</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="89">
-        <f t="shared" si="0"/>
-        <v>1.2271846303085129E-2</v>
-      </c>
-      <c r="I34" s="90" t="str" cm="1">
-        <f t="array" ref="I34">[1]!calcTotCubic(1,16,K34,D34,G34)</f>
-        <v>#HT&lt;4.5!</v>
-      </c>
-      <c r="J34" t="str" cm="1">
-        <f t="array" ref="J34">[1]!calcMerchCubic(1,16,K34,D34,G34,4,0)</f>
-        <v>#HT&lt;4.5!</v>
-      </c>
-      <c r="K34" t="str" cm="1">
-        <f t="array" ref="K34">[1]!VolumeEquationNumber(1,16,1,C34,0)</f>
-        <v>I00FW2W202</v>
-      </c>
+      <c r="H34" s="6"/>
+      <c r="M34" s="84"/>
+      <c r="N34" s="85"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4B9663-1DB5-4381-9887-8746710F68D2}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:P109"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="83" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="83" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" s="86" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6">
+        <v>73</v>
+      </c>
+      <c r="D2" s="7">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>107</v>
+      </c>
+      <c r="H2" s="84">
+        <f t="shared" ref="H2" si="0">(PI() * (D2/2)^2) / 144</f>
+        <v>1.747565455098447</v>
+      </c>
+      <c r="I2" s="85" cm="1">
+        <f t="array" ref="I2">[1]!calcTotCubic(1,16,K2,D2,G2)</f>
+        <v>63.7</v>
+      </c>
+      <c r="J2" cm="1">
+        <f t="array" ref="J2">[1]!calcMerchCubic(1,16,K2,D2,G2,4,0)</f>
+        <v>57.7</v>
+      </c>
+      <c r="K2" t="str" cm="1">
+        <f t="array" ref="K2">[1]!VolumeEquationNumber(1,16,1,C2,0)</f>
+        <v>I00FW2W073</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" cm="1">
+        <f t="array" ref="O2">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N2)</f>
+        <v>20.1937255859375</v>
+      </c>
+      <c r="P2" cm="1">
+        <f t="array" ref="P2">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N2,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>20.1937255859375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" cm="1">
+        <f t="array" ref="O3">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N3)</f>
+        <v>17.88627815246582</v>
+      </c>
+      <c r="P3" cm="1">
+        <f t="array" ref="P3">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N3,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>17.88627815246582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4" cm="1">
+        <f t="array" ref="O4">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N4)</f>
+        <v>16.68548583984375</v>
+      </c>
+      <c r="P4" cm="1">
+        <f t="array" ref="P4">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N4,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>16.68548583984375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5" cm="1">
+        <f t="array" ref="O5">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N5)</f>
+        <v>15.924393653869629</v>
+      </c>
+      <c r="P5" cm="1">
+        <f t="array" ref="P5">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N5,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>15.924393653869629</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6" cm="1">
+        <f t="array" ref="O6">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N6)</f>
+        <v>15.396261215209961</v>
+      </c>
+      <c r="P6" cm="1">
+        <f t="array" ref="P6">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N6,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>15.396261215209961</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7" cm="1">
+        <f t="array" ref="O7">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N7)</f>
+        <v>15.009604454040527</v>
+      </c>
+      <c r="P7" cm="1">
+        <f t="array" ref="P7">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N7,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>15.009604454040527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8" cm="1">
+        <f t="array" ref="O8">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N8)</f>
+        <v>14.715923309326172</v>
+      </c>
+      <c r="P8" cm="1">
+        <f t="array" ref="P8">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N8,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>14.715923309326172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9" cm="1">
+        <f t="array" ref="O9">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N9)</f>
+        <v>14.486467361450195</v>
+      </c>
+      <c r="P9" cm="1">
+        <f t="array" ref="P9">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N9,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>14.486467361450195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10" cm="1">
+        <f t="array" ref="O10">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N10)</f>
+        <v>14.302850723266602</v>
+      </c>
+      <c r="P10" cm="1">
+        <f t="array" ref="P10">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N10,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>14.302850723266602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>9</v>
+      </c>
+      <c r="O11" cm="1">
+        <f t="array" ref="O11">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N11)</f>
+        <v>14.152651786804199</v>
+      </c>
+      <c r="P11" cm="1">
+        <f t="array" ref="P11">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N11,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>14.152651786804199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12" cm="1">
+        <f t="array" ref="O12">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N12)</f>
+        <v>14.027126312255859</v>
+      </c>
+      <c r="P12" cm="1">
+        <f t="array" ref="P12">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N12,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>14.027126312255859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>11</v>
+      </c>
+      <c r="O13" cm="1">
+        <f t="array" ref="O13">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N13)</f>
+        <v>13.919919967651367</v>
+      </c>
+      <c r="P13" cm="1">
+        <f t="array" ref="P13">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N13,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.919919967651367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>12</v>
+      </c>
+      <c r="O14" cm="1">
+        <f t="array" ref="O14">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N14)</f>
+        <v>13.826301574707031</v>
+      </c>
+      <c r="P14" cm="1">
+        <f t="array" ref="P14">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N14,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.826301574707031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>13</v>
+      </c>
+      <c r="O15" cm="1">
+        <f t="array" ref="O15">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N15)</f>
+        <v>13.742681503295898</v>
+      </c>
+      <c r="P15" cm="1">
+        <f t="array" ref="P15">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N15,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.742681503295898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>14</v>
+      </c>
+      <c r="O16" cm="1">
+        <f t="array" ref="O16">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N16)</f>
+        <v>13.666291236877441</v>
+      </c>
+      <c r="P16" cm="1">
+        <f t="array" ref="P16">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N16,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.666291236877441</v>
+      </c>
+    </row>
+    <row r="17" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>15</v>
+      </c>
+      <c r="O17" cm="1">
+        <f t="array" ref="O17">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N17)</f>
+        <v>13.594975471496582</v>
+      </c>
+      <c r="P17" cm="1">
+        <f t="array" ref="P17">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N17,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.594975471496582</v>
+      </c>
+    </row>
+    <row r="18" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>16</v>
+      </c>
+      <c r="O18" cm="1">
+        <f t="array" ref="O18">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N18)</f>
+        <v>13.527040481567383</v>
+      </c>
+      <c r="P18" cm="1">
+        <f t="array" ref="P18">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N18,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.527040481567383</v>
+      </c>
+    </row>
+    <row r="19" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>17</v>
+      </c>
+      <c r="O19" cm="1">
+        <f t="array" ref="O19">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N19)</f>
+        <v>13.461148262023926</v>
+      </c>
+      <c r="P19" cm="1">
+        <f t="array" ref="P19">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N19,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.461148262023926</v>
+      </c>
+    </row>
+    <row r="20" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>18</v>
+      </c>
+      <c r="O20" cm="1">
+        <f t="array" ref="O20">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N20)</f>
+        <v>13.396241188049316</v>
+      </c>
+      <c r="P20" cm="1">
+        <f t="array" ref="P20">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N20,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.396241188049316</v>
+      </c>
+    </row>
+    <row r="21" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>19</v>
+      </c>
+      <c r="O21" cm="1">
+        <f t="array" ref="O21">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N21)</f>
+        <v>13.33154296875</v>
+      </c>
+      <c r="P21" cm="1">
+        <f t="array" ref="P21">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N21,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.33154296875</v>
+      </c>
+    </row>
+    <row r="22" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>20</v>
+      </c>
+      <c r="O22" cm="1">
+        <f t="array" ref="O22">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N22)</f>
+        <v>13.266825675964355</v>
+      </c>
+      <c r="P22" cm="1">
+        <f t="array" ref="P22">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N22,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.266825675964355</v>
+      </c>
+    </row>
+    <row r="23" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>21</v>
+      </c>
+      <c r="O23" cm="1">
+        <f t="array" ref="O23">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N23)</f>
+        <v>13.202018737792969</v>
+      </c>
+      <c r="P23" cm="1">
+        <f t="array" ref="P23">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N23,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.202018737792969</v>
+      </c>
+    </row>
+    <row r="24" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>22</v>
+      </c>
+      <c r="O24" cm="1">
+        <f t="array" ref="O24">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N24)</f>
+        <v>13.13704776763916</v>
+      </c>
+      <c r="P24" cm="1">
+        <f t="array" ref="P24">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N24,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.13704776763916</v>
+      </c>
+    </row>
+    <row r="25" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>23</v>
+      </c>
+      <c r="O25" cm="1">
+        <f t="array" ref="O25">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N25)</f>
+        <v>13.071834564208984</v>
+      </c>
+      <c r="P25" cm="1">
+        <f t="array" ref="P25">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N25,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.071834564208984</v>
+      </c>
+    </row>
+    <row r="26" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>24</v>
+      </c>
+      <c r="O26" cm="1">
+        <f t="array" ref="O26">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N26)</f>
+        <v>13.006305694580078</v>
+      </c>
+      <c r="P26" cm="1">
+        <f t="array" ref="P26">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N26,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>13.006305694580078</v>
+      </c>
+    </row>
+    <row r="27" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>25</v>
+      </c>
+      <c r="O27" cm="1">
+        <f t="array" ref="O27">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N27)</f>
+        <v>12.940382957458496</v>
+      </c>
+      <c r="P27" cm="1">
+        <f t="array" ref="P27">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N27,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.940382957458496</v>
+      </c>
+    </row>
+    <row r="28" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>26</v>
+      </c>
+      <c r="O28" cm="1">
+        <f t="array" ref="O28">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N28)</f>
+        <v>12.873992919921875</v>
+      </c>
+      <c r="P28" cm="1">
+        <f t="array" ref="P28">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N28,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.873992919921875</v>
+      </c>
+    </row>
+    <row r="29" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>27</v>
+      </c>
+      <c r="O29" cm="1">
+        <f t="array" ref="O29">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N29)</f>
+        <v>12.807058334350586</v>
+      </c>
+      <c r="P29" cm="1">
+        <f t="array" ref="P29">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N29,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.807058334350586</v>
+      </c>
+    </row>
+    <row r="30" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>28</v>
+      </c>
+      <c r="O30" cm="1">
+        <f t="array" ref="O30">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N30)</f>
+        <v>12.739502906799316</v>
+      </c>
+      <c r="P30" cm="1">
+        <f t="array" ref="P30">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N30,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.739502906799316</v>
+      </c>
+    </row>
+    <row r="31" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>29</v>
+      </c>
+      <c r="O31" cm="1">
+        <f t="array" ref="O31">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N31)</f>
+        <v>12.671252250671387</v>
+      </c>
+      <c r="P31" cm="1">
+        <f t="array" ref="P31">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N31,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.671252250671387</v>
+      </c>
+    </row>
+    <row r="32" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>30</v>
+      </c>
+      <c r="O32" cm="1">
+        <f t="array" ref="O32">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N32)</f>
+        <v>12.602229118347168</v>
+      </c>
+      <c r="P32" cm="1">
+        <f t="array" ref="P32">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N32,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.602229118347168</v>
+      </c>
+    </row>
+    <row r="33" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>31</v>
+      </c>
+      <c r="O33" cm="1">
+        <f t="array" ref="O33">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N33)</f>
+        <v>12.532358169555664</v>
+      </c>
+      <c r="P33" cm="1">
+        <f t="array" ref="P33">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N33,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.532358169555664</v>
+      </c>
+    </row>
+    <row r="34" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>32</v>
+      </c>
+      <c r="O34" cm="1">
+        <f t="array" ref="O34">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N34)</f>
+        <v>12.461565017700195</v>
+      </c>
+      <c r="P34" cm="1">
+        <f t="array" ref="P34">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N34,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.461565017700195</v>
+      </c>
+    </row>
+    <row r="35" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>33</v>
+      </c>
+      <c r="O35" cm="1">
+        <f t="array" ref="O35">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N35)</f>
+        <v>12.389771461486816</v>
+      </c>
+      <c r="P35" cm="1">
+        <f t="array" ref="P35">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N35,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.389771461486816</v>
+      </c>
+    </row>
+    <row r="36" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>34</v>
+      </c>
+      <c r="O36" cm="1">
+        <f t="array" ref="O36">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N36)</f>
+        <v>12.316902160644531</v>
+      </c>
+      <c r="P36" cm="1">
+        <f t="array" ref="P36">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N36,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.316902160644531</v>
+      </c>
+    </row>
+    <row r="37" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>35</v>
+      </c>
+      <c r="O37" cm="1">
+        <f t="array" ref="O37">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N37)</f>
+        <v>12.24288272857666</v>
+      </c>
+      <c r="P37" cm="1">
+        <f t="array" ref="P37">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N37,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.24288272857666</v>
+      </c>
+    </row>
+    <row r="38" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>36</v>
+      </c>
+      <c r="O38" cm="1">
+        <f t="array" ref="O38">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N38)</f>
+        <v>12.167635917663574</v>
+      </c>
+      <c r="P38" cm="1">
+        <f t="array" ref="P38">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N38,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.167635917663574</v>
+      </c>
+    </row>
+    <row r="39" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>37</v>
+      </c>
+      <c r="O39" cm="1">
+        <f t="array" ref="O39">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N39)</f>
+        <v>12.091087341308594</v>
+      </c>
+      <c r="P39" cm="1">
+        <f t="array" ref="P39">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N39,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.091087341308594</v>
+      </c>
+    </row>
+    <row r="40" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>38</v>
+      </c>
+      <c r="O40" cm="1">
+        <f t="array" ref="O40">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N40)</f>
+        <v>12.013160705566406</v>
+      </c>
+      <c r="P40" cm="1">
+        <f t="array" ref="P40">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N40,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>12.013160705566406</v>
+      </c>
+    </row>
+    <row r="41" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>39</v>
+      </c>
+      <c r="O41" cm="1">
+        <f t="array" ref="O41">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N41)</f>
+        <v>11.933779716491699</v>
+      </c>
+      <c r="P41" cm="1">
+        <f t="array" ref="P41">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N41,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.933779716491699</v>
+      </c>
+    </row>
+    <row r="42" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>40</v>
+      </c>
+      <c r="O42" cm="1">
+        <f t="array" ref="O42">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N42)</f>
+        <v>11.852869033813477</v>
+      </c>
+      <c r="P42" cm="1">
+        <f t="array" ref="P42">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N42,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.852869033813477</v>
+      </c>
+    </row>
+    <row r="43" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <v>41</v>
+      </c>
+      <c r="O43" cm="1">
+        <f t="array" ref="O43">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N43)</f>
+        <v>11.770353317260742</v>
+      </c>
+      <c r="P43" cm="1">
+        <f t="array" ref="P43">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N43,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.770353317260742</v>
+      </c>
+    </row>
+    <row r="44" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>42</v>
+      </c>
+      <c r="O44" cm="1">
+        <f t="array" ref="O44">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N44)</f>
+        <v>11.6861572265625</v>
+      </c>
+      <c r="P44" cm="1">
+        <f t="array" ref="P44">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N44,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.6861572265625</v>
+      </c>
+    </row>
+    <row r="45" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <v>43</v>
+      </c>
+      <c r="O45" cm="1">
+        <f t="array" ref="O45">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N45)</f>
+        <v>11.60020637512207</v>
+      </c>
+      <c r="P45" cm="1">
+        <f t="array" ref="P45">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N45,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.60020637512207</v>
+      </c>
+    </row>
+    <row r="46" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <v>44</v>
+      </c>
+      <c r="O46" cm="1">
+        <f t="array" ref="O46">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N46)</f>
+        <v>11.512423515319824</v>
+      </c>
+      <c r="P46" cm="1">
+        <f t="array" ref="P46">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N46,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.512423515319824</v>
+      </c>
+    </row>
+    <row r="47" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>45</v>
+      </c>
+      <c r="O47" cm="1">
+        <f t="array" ref="O47">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N47)</f>
+        <v>11.422735214233398</v>
+      </c>
+      <c r="P47" cm="1">
+        <f t="array" ref="P47">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N47,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.422735214233398</v>
+      </c>
+    </row>
+    <row r="48" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>46</v>
+      </c>
+      <c r="O48" cm="1">
+        <f t="array" ref="O48">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N48)</f>
+        <v>11.331066131591797</v>
+      </c>
+      <c r="P48" cm="1">
+        <f t="array" ref="P48">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N48,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.331066131591797</v>
+      </c>
+    </row>
+    <row r="49" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>47</v>
+      </c>
+      <c r="O49" cm="1">
+        <f t="array" ref="O49">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N49)</f>
+        <v>11.23734188079834</v>
+      </c>
+      <c r="P49" cm="1">
+        <f t="array" ref="P49">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N49,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.23734188079834</v>
+      </c>
+    </row>
+    <row r="50" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>48</v>
+      </c>
+      <c r="O50" cm="1">
+        <f t="array" ref="O50">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N50)</f>
+        <v>11.141488075256348</v>
+      </c>
+      <c r="P50" cm="1">
+        <f t="array" ref="P50">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N50,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.141488075256348</v>
+      </c>
+    </row>
+    <row r="51" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>49</v>
+      </c>
+      <c r="O51" cm="1">
+        <f t="array" ref="O51">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N51)</f>
+        <v>11.043429374694824</v>
+      </c>
+      <c r="P51" cm="1">
+        <f t="array" ref="P51">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N51,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>11.043429374694824</v>
+      </c>
+    </row>
+    <row r="52" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <v>50</v>
+      </c>
+      <c r="O52" cm="1">
+        <f t="array" ref="O52">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N52)</f>
+        <v>10.943093299865723</v>
+      </c>
+      <c r="P52" cm="1">
+        <f t="array" ref="P52">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N52,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.943093299865723</v>
+      </c>
+    </row>
+    <row r="53" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <v>51</v>
+      </c>
+      <c r="O53" cm="1">
+        <f t="array" ref="O53">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N53)</f>
+        <v>10.840405464172363</v>
+      </c>
+      <c r="P53" cm="1">
+        <f t="array" ref="P53">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N53,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.840405464172363</v>
+      </c>
+    </row>
+    <row r="54" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <v>52</v>
+      </c>
+      <c r="O54" cm="1">
+        <f t="array" ref="O54">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N54)</f>
+        <v>10.735294342041016</v>
+      </c>
+      <c r="P54" cm="1">
+        <f t="array" ref="P54">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N54,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.735294342041016</v>
+      </c>
+    </row>
+    <row r="55" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <v>53</v>
+      </c>
+      <c r="O55" cm="1">
+        <f t="array" ref="O55">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N55)</f>
+        <v>10.627686500549316</v>
+      </c>
+      <c r="P55" cm="1">
+        <f t="array" ref="P55">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N55,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.627686500549316</v>
+      </c>
+    </row>
+    <row r="56" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <v>54</v>
+      </c>
+      <c r="O56" cm="1">
+        <f t="array" ref="O56">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N56)</f>
+        <v>10.517511367797852</v>
+      </c>
+      <c r="P56" cm="1">
+        <f t="array" ref="P56">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N56,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.517511367797852</v>
+      </c>
+    </row>
+    <row r="57" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>55</v>
+      </c>
+      <c r="O57" cm="1">
+        <f t="array" ref="O57">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N57)</f>
+        <v>10.404695510864258</v>
+      </c>
+      <c r="P57" cm="1">
+        <f t="array" ref="P57">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N57,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.404695510864258</v>
+      </c>
+    </row>
+    <row r="58" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <v>56</v>
+      </c>
+      <c r="O58" cm="1">
+        <f t="array" ref="O58">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N58)</f>
+        <v>10.289169311523438</v>
+      </c>
+      <c r="P58" cm="1">
+        <f t="array" ref="P58">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N58,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.289169311523438</v>
+      </c>
+    </row>
+    <row r="59" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N59">
+        <v>57</v>
+      </c>
+      <c r="O59" cm="1">
+        <f t="array" ref="O59">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N59)</f>
+        <v>10.170864105224609</v>
+      </c>
+      <c r="P59" cm="1">
+        <f t="array" ref="P59">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N59,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.170864105224609</v>
+      </c>
+    </row>
+    <row r="60" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N60">
+        <v>58</v>
+      </c>
+      <c r="O60" cm="1">
+        <f t="array" ref="O60">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N60)</f>
+        <v>10.049708366394043</v>
+      </c>
+      <c r="P60" cm="1">
+        <f t="array" ref="P60">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N60,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>10.049708366394043</v>
+      </c>
+    </row>
+    <row r="61" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N61">
+        <v>59</v>
+      </c>
+      <c r="O61" cm="1">
+        <f t="array" ref="O61">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N61)</f>
+        <v>9.9256381988525391</v>
+      </c>
+      <c r="P61" cm="1">
+        <f t="array" ref="P61">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N61,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>9.9256381988525391</v>
+      </c>
+    </row>
+    <row r="62" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N62">
+        <v>60</v>
+      </c>
+      <c r="O62" cm="1">
+        <f t="array" ref="O62">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N62)</f>
+        <v>9.7985820770263672</v>
+      </c>
+      <c r="P62" cm="1">
+        <f t="array" ref="P62">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N62,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>9.7985820770263672</v>
+      </c>
+    </row>
+    <row r="63" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N63">
+        <v>61</v>
+      </c>
+      <c r="O63" cm="1">
+        <f t="array" ref="O63">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N63)</f>
+        <v>9.6684789657592773</v>
+      </c>
+      <c r="P63" cm="1">
+        <f t="array" ref="P63">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N63,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>9.6684789657592773</v>
+      </c>
+    </row>
+    <row r="64" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N64">
+        <v>62</v>
+      </c>
+      <c r="O64" cm="1">
+        <f t="array" ref="O64">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N64)</f>
+        <v>9.5352621078491211</v>
+      </c>
+      <c r="P64" cm="1">
+        <f t="array" ref="P64">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N64,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>9.5352621078491211</v>
+      </c>
+    </row>
+    <row r="65" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N65">
+        <v>63</v>
+      </c>
+      <c r="O65" cm="1">
+        <f t="array" ref="O65">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N65)</f>
+        <v>9.3988685607910156</v>
+      </c>
+      <c r="P65" cm="1">
+        <f t="array" ref="P65">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N65,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>9.3988685607910156</v>
+      </c>
+    </row>
+    <row r="66" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N66">
+        <v>64</v>
+      </c>
+      <c r="O66" cm="1">
+        <f t="array" ref="O66">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N66)</f>
+        <v>9.2592391967773438</v>
+      </c>
+      <c r="P66" cm="1">
+        <f t="array" ref="P66">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N66,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>9.2592391967773438</v>
+      </c>
+    </row>
+    <row r="67" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N67">
+        <v>65</v>
+      </c>
+      <c r="O67" cm="1">
+        <f t="array" ref="O67">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N67)</f>
+        <v>9.1163120269775391</v>
+      </c>
+      <c r="P67" cm="1">
+        <f t="array" ref="P67">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N67,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>9.1163120269775391</v>
+      </c>
+    </row>
+    <row r="68" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N68">
+        <v>66</v>
+      </c>
+      <c r="O68" cm="1">
+        <f t="array" ref="O68">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N68)</f>
+        <v>8.9700326919555664</v>
+      </c>
+      <c r="P68" cm="1">
+        <f t="array" ref="P68">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N68,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>8.9700326919555664</v>
+      </c>
+    </row>
+    <row r="69" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N69">
+        <v>67</v>
+      </c>
+      <c r="O69" cm="1">
+        <f t="array" ref="O69">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N69)</f>
+        <v>8.820343017578125</v>
+      </c>
+      <c r="P69" cm="1">
+        <f t="array" ref="P69">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N69,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>8.820343017578125</v>
+      </c>
+    </row>
+    <row r="70" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N70">
+        <v>68</v>
+      </c>
+      <c r="O70" cm="1">
+        <f t="array" ref="O70">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N70)</f>
+        <v>8.6671943664550781</v>
+      </c>
+      <c r="P70" cm="1">
+        <f t="array" ref="P70">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N70,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>8.6671943664550781</v>
+      </c>
+    </row>
+    <row r="71" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N71">
+        <v>69</v>
+      </c>
+      <c r="O71" cm="1">
+        <f t="array" ref="O71">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N71)</f>
+        <v>8.5105323791503906</v>
+      </c>
+      <c r="P71" cm="1">
+        <f t="array" ref="P71">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N71,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>8.5105323791503906</v>
+      </c>
+    </row>
+    <row r="72" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <v>70</v>
+      </c>
+      <c r="O72" cm="1">
+        <f t="array" ref="O72">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N72)</f>
+        <v>8.3503103256225586</v>
+      </c>
+      <c r="P72" cm="1">
+        <f t="array" ref="P72">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N72,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>8.3503103256225586</v>
+      </c>
+    </row>
+    <row r="73" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <v>71</v>
+      </c>
+      <c r="O73" cm="1">
+        <f t="array" ref="O73">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N73)</f>
+        <v>8.1864862442016602</v>
+      </c>
+      <c r="P73" cm="1">
+        <f t="array" ref="P73">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N73,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>8.1864862442016602</v>
+      </c>
+    </row>
+    <row r="74" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N74">
+        <v>72</v>
+      </c>
+      <c r="O74" cm="1">
+        <f t="array" ref="O74">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N74)</f>
+        <v>8.0190153121948242</v>
+      </c>
+      <c r="P74" cm="1">
+        <f t="array" ref="P74">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N74,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>8.0190153121948242</v>
+      </c>
+    </row>
+    <row r="75" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <v>73</v>
+      </c>
+      <c r="O75" cm="1">
+        <f t="array" ref="O75">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N75)</f>
+        <v>7.8478631973266602</v>
+      </c>
+      <c r="P75" cm="1">
+        <f t="array" ref="P75">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N75,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>7.8478631973266602</v>
+      </c>
+    </row>
+    <row r="76" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N76">
+        <v>74</v>
+      </c>
+      <c r="O76" cm="1">
+        <f t="array" ref="O76">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N76)</f>
+        <v>7.6729946136474609</v>
+      </c>
+      <c r="P76" cm="1">
+        <f t="array" ref="P76">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N76,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>7.6729946136474609</v>
+      </c>
+    </row>
+    <row r="77" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N77">
+        <v>75</v>
+      </c>
+      <c r="O77" cm="1">
+        <f t="array" ref="O77">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N77)</f>
+        <v>7.4943790435791016</v>
+      </c>
+      <c r="P77" cm="1">
+        <f t="array" ref="P77">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N77,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>7.4943790435791016</v>
+      </c>
+    </row>
+    <row r="78" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N78">
+        <v>76</v>
+      </c>
+      <c r="O78" cm="1">
+        <f t="array" ref="O78">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N78)</f>
+        <v>7.3119931221008301</v>
+      </c>
+      <c r="P78" cm="1">
+        <f t="array" ref="P78">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N78,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>7.3119931221008301</v>
+      </c>
+    </row>
+    <row r="79" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N79">
+        <v>77</v>
+      </c>
+      <c r="O79" cm="1">
+        <f t="array" ref="O79">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N79)</f>
+        <v>7.1258144378662109</v>
+      </c>
+      <c r="P79" cm="1">
+        <f t="array" ref="P79">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N79,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>7.1258144378662109</v>
+      </c>
+    </row>
+    <row r="80" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N80">
+        <v>78</v>
+      </c>
+      <c r="O80" cm="1">
+        <f t="array" ref="O80">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N80)</f>
+        <v>6.9358291625976563</v>
+      </c>
+      <c r="P80" cm="1">
+        <f t="array" ref="P80">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N80,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>6.9358291625976563</v>
+      </c>
+    </row>
+    <row r="81" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N81">
+        <v>79</v>
+      </c>
+      <c r="O81" cm="1">
+        <f t="array" ref="O81">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N81)</f>
+        <v>6.7420282363891602</v>
+      </c>
+      <c r="P81" cm="1">
+        <f t="array" ref="P81">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N81,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>6.7420282363891602</v>
+      </c>
+    </row>
+    <row r="82" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N82">
+        <v>80</v>
+      </c>
+      <c r="O82" cm="1">
+        <f t="array" ref="O82">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N82)</f>
+        <v>6.5444040298461914</v>
+      </c>
+      <c r="P82" cm="1">
+        <f t="array" ref="P82">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N82,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>6.5444040298461914</v>
+      </c>
+    </row>
+    <row r="83" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N83">
+        <v>81</v>
+      </c>
+      <c r="O83" cm="1">
+        <f t="array" ref="O83">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N83)</f>
+        <v>6.3429622650146484</v>
+      </c>
+      <c r="P83" cm="1">
+        <f t="array" ref="P83">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N83,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>6.3429622650146484</v>
+      </c>
+    </row>
+    <row r="84" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N84">
+        <v>82</v>
+      </c>
+      <c r="O84" cm="1">
+        <f t="array" ref="O84">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N84)</f>
+        <v>6.1377100944519043</v>
+      </c>
+      <c r="P84" cm="1">
+        <f t="array" ref="P84">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N84,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>6.1377100944519043</v>
+      </c>
+    </row>
+    <row r="85" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N85">
+        <v>83</v>
+      </c>
+      <c r="O85" cm="1">
+        <f t="array" ref="O85">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N85)</f>
+        <v>5.9286661148071289</v>
+      </c>
+      <c r="P85" cm="1">
+        <f t="array" ref="P85">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N85,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>5.9286661148071289</v>
+      </c>
+    </row>
+    <row r="86" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N86">
+        <v>84</v>
+      </c>
+      <c r="O86" cm="1">
+        <f t="array" ref="O86">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N86)</f>
+        <v>5.7158517837524414</v>
+      </c>
+      <c r="P86" cm="1">
+        <f t="array" ref="P86">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N86,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>5.7158517837524414</v>
+      </c>
+    </row>
+    <row r="87" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N87">
+        <v>85</v>
+      </c>
+      <c r="O87" cm="1">
+        <f t="array" ref="O87">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N87)</f>
+        <v>5.4993019104003906</v>
+      </c>
+      <c r="P87" cm="1">
+        <f t="array" ref="P87">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N87,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>5.4993019104003906</v>
+      </c>
+    </row>
+    <row r="88" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N88">
+        <v>86</v>
+      </c>
+      <c r="O88" cm="1">
+        <f t="array" ref="O88">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N88)</f>
+        <v>5.2790560722351074</v>
+      </c>
+      <c r="P88" cm="1">
+        <f t="array" ref="P88">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N88,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>5.2790560722351074</v>
+      </c>
+    </row>
+    <row r="89" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N89">
+        <v>87</v>
+      </c>
+      <c r="O89" cm="1">
+        <f t="array" ref="O89">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N89)</f>
+        <v>5.0551638603210449</v>
+      </c>
+      <c r="P89" cm="1">
+        <f t="array" ref="P89">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N89,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>5.0551638603210449</v>
+      </c>
+    </row>
+    <row r="90" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N90">
+        <v>88</v>
+      </c>
+      <c r="O90" cm="1">
+        <f t="array" ref="O90">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N90)</f>
+        <v>4.8276877403259277</v>
+      </c>
+      <c r="P90" cm="1">
+        <f t="array" ref="P90">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N90,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>4.8276877403259277</v>
+      </c>
+    </row>
+    <row r="91" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N91">
+        <v>89</v>
+      </c>
+      <c r="O91" cm="1">
+        <f t="array" ref="O91">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N91)</f>
+        <v>4.5966958999633789</v>
+      </c>
+      <c r="P91" cm="1">
+        <f t="array" ref="P91">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N91,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>4.5966958999633789</v>
+      </c>
+    </row>
+    <row r="92" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N92">
+        <v>90</v>
+      </c>
+      <c r="O92" cm="1">
+        <f t="array" ref="O92">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N92)</f>
+        <v>4.3622736930847168</v>
+      </c>
+      <c r="P92" cm="1">
+        <f t="array" ref="P92">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N92,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>4.3622736930847168</v>
+      </c>
+    </row>
+    <row r="93" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N93">
+        <v>91</v>
+      </c>
+      <c r="O93" cm="1">
+        <f t="array" ref="O93">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N93)</f>
+        <v>4.12451171875</v>
+      </c>
+      <c r="P93" cm="1">
+        <f t="array" ref="P93">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N93,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>4.12451171875</v>
+      </c>
+    </row>
+    <row r="94" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N94">
+        <v>92</v>
+      </c>
+      <c r="O94" cm="1">
+        <f t="array" ref="O94">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N94)</f>
+        <v>3.8835158348083496</v>
+      </c>
+      <c r="P94" cm="1">
+        <f t="array" ref="P94">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N94,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>3.8835158348083496</v>
+      </c>
+    </row>
+    <row r="95" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N95">
+        <v>93</v>
+      </c>
+      <c r="O95" cm="1">
+        <f t="array" ref="O95">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N95)</f>
+        <v>3.6394081115722656</v>
+      </c>
+      <c r="P95" cm="1">
+        <f t="array" ref="P95">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N95,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>3.6394081115722656</v>
+      </c>
+    </row>
+    <row r="96" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N96">
+        <v>94</v>
+      </c>
+      <c r="O96" cm="1">
+        <f t="array" ref="O96">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N96)</f>
+        <v>3.3923192024230957</v>
+      </c>
+      <c r="P96" cm="1">
+        <f t="array" ref="P96">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N96,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>3.3923192024230957</v>
+      </c>
+    </row>
+    <row r="97" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N97">
+        <v>95</v>
+      </c>
+      <c r="O97" cm="1">
+        <f t="array" ref="O97">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N97)</f>
+        <v>3.1424002647399902</v>
+      </c>
+      <c r="P97" cm="1">
+        <f t="array" ref="P97">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N97,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>3.1424002647399902</v>
+      </c>
+    </row>
+    <row r="98" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N98">
+        <v>96</v>
+      </c>
+      <c r="O98" cm="1">
+        <f t="array" ref="O98">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N98)</f>
+        <v>2.8898136615753174</v>
+      </c>
+      <c r="P98" cm="1">
+        <f t="array" ref="P98">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N98,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>2.8898136615753174</v>
+      </c>
+    </row>
+    <row r="99" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N99">
+        <v>97</v>
+      </c>
+      <c r="O99" cm="1">
+        <f t="array" ref="O99">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N99)</f>
+        <v>2.6347389221191406</v>
+      </c>
+      <c r="P99" cm="1">
+        <f t="array" ref="P99">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N99,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>2.6347389221191406</v>
+      </c>
+    </row>
+    <row r="100" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N100">
+        <v>98</v>
+      </c>
+      <c r="O100" cm="1">
+        <f t="array" ref="O100">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N100)</f>
+        <v>2.3773760795593262</v>
+      </c>
+      <c r="P100" cm="1">
+        <f t="array" ref="P100">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N100,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>2.3773760795593262</v>
+      </c>
+    </row>
+    <row r="101" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N101">
+        <v>99</v>
+      </c>
+      <c r="O101" cm="1">
+        <f t="array" ref="O101">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N101)</f>
+        <v>2.117938756942749</v>
+      </c>
+      <c r="P101" cm="1">
+        <f t="array" ref="P101">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N101,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>2.117938756942749</v>
+      </c>
+    </row>
+    <row r="102" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N102">
+        <v>100</v>
+      </c>
+      <c r="O102" cm="1">
+        <f t="array" ref="O102">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N102)</f>
+        <v>1.8566651344299316</v>
+      </c>
+      <c r="P102" cm="1">
+        <f t="array" ref="P102">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N102,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>1.8566651344299316</v>
+      </c>
+    </row>
+    <row r="103" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N103">
+        <v>101</v>
+      </c>
+      <c r="O103" cm="1">
+        <f t="array" ref="O103">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N103)</f>
+        <v>1.5938084125518799</v>
+      </c>
+      <c r="P103" cm="1">
+        <f t="array" ref="P103">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N103,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>1.5938084125518799</v>
+      </c>
+    </row>
+    <row r="104" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N104">
+        <v>102</v>
+      </c>
+      <c r="O104" cm="1">
+        <f t="array" ref="O104">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N104)</f>
+        <v>1.3296496868133545</v>
+      </c>
+      <c r="P104" cm="1">
+        <f t="array" ref="P104">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N104,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>1.3296496868133545</v>
+      </c>
+    </row>
+    <row r="105" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N105">
+        <v>103</v>
+      </c>
+      <c r="O105" cm="1">
+        <f t="array" ref="O105">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N105)</f>
+        <v>1.0644845962524414</v>
+      </c>
+      <c r="P105" cm="1">
+        <f t="array" ref="P105">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N105,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>1.0644845962524414</v>
+      </c>
+    </row>
+    <row r="106" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N106">
+        <v>104</v>
+      </c>
+      <c r="O106" cm="1">
+        <f t="array" ref="O106">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N106)</f>
+        <v>0.79863625764846802</v>
+      </c>
+      <c r="P106" cm="1">
+        <f t="array" ref="P106">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N106,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>0.79863625764846802</v>
+      </c>
+    </row>
+    <row r="107" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N107">
+        <v>105</v>
+      </c>
+      <c r="O107" cm="1">
+        <f t="array" ref="O107">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N107)</f>
+        <v>0.5324552059173584</v>
+      </c>
+      <c r="P107" cm="1">
+        <f t="array" ref="P107">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N107,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>0.5324552059173584</v>
+      </c>
+    </row>
+    <row r="108" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N108">
+        <v>106</v>
+      </c>
+      <c r="O108" cm="1">
+        <f t="array" ref="O108">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N108)</f>
+        <v>0.26622676849365234</v>
+      </c>
+      <c r="P108" cm="1">
+        <f t="array" ref="P108">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N108,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>0.26622676849365234</v>
+      </c>
+    </row>
+    <row r="109" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N109">
+        <v>107</v>
+      </c>
+      <c r="O109" cm="1">
+        <f t="array" ref="O109">[1]!calcDib(1,16,$K$2,$D$2,$G$2,N109)</f>
+        <v>0</v>
+      </c>
+      <c r="P109" cm="1">
+        <f t="array" ref="P109">[2]!getDibAdv(1,16,$K$2,$D$2,$G$2,N109,0,0,0,0,0,0,0,0,0,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FFA481-BCE4-4227-A804-DCC87E6D4A9E}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P106"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3218,10 +5912,10 @@
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84"/>
+      <c r="G2" s="88"/>
       <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
@@ -3247,14 +5941,14 @@
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="L3" s="85" t="s">
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="O3" s="85" t="s">
+      <c r="M3" s="89"/>
+      <c r="O3" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="85"/>
+      <c r="P3" s="89"/>
     </row>
     <row r="4" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
@@ -3269,10 +5963,10 @@
       <c r="E4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="87"/>
+      <c r="G4" s="91"/>
       <c r="I4" s="19" t="s">
         <v>15</v>
       </c>
@@ -5429,8 +8123,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B464DCD8-2AB7-4A5C-8684-F40AFC0D2027}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>